<commit_message>
Adding support for irregular nouns
</commit_message>
<xml_diff>
--- a/data/tables/paradigms.xlsx
+++ b/data/tables/paradigms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://havas-my.sharepoint.com/personal/jaime_garcia_globalservs_com/Documents/Desktop/Proyectos/Personal/TsakonianDB/data/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{78C97BE1-9217-4986-ACE4-9B93006B3430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A68CE17-5859-489A-AF2D-1A83247276C9}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="13_ncr:1_{78C97BE1-9217-4986-ACE4-9B93006B3430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57B354F1-9681-4D23-811E-C156F06A7FA7}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="114">
   <si>
     <t>notes</t>
   </si>
@@ -265,6 +265,108 @@
   </si>
   <si>
     <t>ίου</t>
+  </si>
+  <si>
+    <t>γέρου</t>
+  </si>
+  <si>
+    <t>γέροι</t>
+  </si>
+  <si>
+    <t>αθή</t>
+  </si>
+  <si>
+    <t>αθήνε</t>
+  </si>
+  <si>
+    <t>ούθι</t>
+  </si>
+  <si>
+    <t>ουθίουνε</t>
+  </si>
+  <si>
+    <t>ψιλέ</t>
+  </si>
+  <si>
+    <t>ψιού</t>
+  </si>
+  <si>
+    <t>ψιλ̣οί</t>
+  </si>
+  <si>
+    <t>κούε</t>
+  </si>
+  <si>
+    <t>κουνέ</t>
+  </si>
+  <si>
+    <t>κούν̇οι</t>
+  </si>
+  <si>
+    <t>άμπελε</t>
+  </si>
+  <si>
+    <t>μάτη</t>
+  </si>
+  <si>
+    <t>μάτη / ματερί</t>
+  </si>
+  <si>
+    <t>ματέρε</t>
+  </si>
+  <si>
+    <t>σάτη</t>
+  </si>
+  <si>
+    <t>σάτη / σατερί</t>
+  </si>
+  <si>
+    <t>σατέρε</t>
+  </si>
+  <si>
+    <t>άμπελε / άμπελ̣ή</t>
+  </si>
+  <si>
+    <t>κρόπο</t>
+  </si>
+  <si>
+    <t>κρόπε</t>
+  </si>
+  <si>
+    <t>κόκαλε</t>
+  </si>
+  <si>
+    <t>κόκα</t>
+  </si>
+  <si>
+    <t>τσ̌έρβουλε</t>
+  </si>
+  <si>
+    <t>τσ̌έρβα</t>
+  </si>
+  <si>
+    <t>π̇ιτόκαλε</t>
+  </si>
+  <si>
+    <t>π̇ιτόκα</t>
+  </si>
+  <si>
+    <t>κάλ̣ι</t>
+  </si>
+  <si>
+    <t>κάβα</t>
+  </si>
+  <si>
+    <t>μάλ̣ι</t>
+  </si>
+  <si>
+    <t>μάβα</t>
+  </si>
+  <si>
+    <t>άι</t>
+  </si>
+  <si>
+    <t>άζα</t>
   </si>
 </sst>
 </file>
@@ -420,8 +522,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C24BDC91-46F2-4EBF-B033-8809523F8BB9}" name="Tabla2" displayName="Tabla2" ref="A1:D32" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D32" xr:uid="{C24BDC91-46F2-4EBF-B033-8809523F8BB9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C24BDC91-46F2-4EBF-B033-8809523F8BB9}" name="Tabla2" displayName="Tabla2" ref="A1:D47" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D47" xr:uid="{C24BDC91-46F2-4EBF-B033-8809523F8BB9}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{C1DD779A-CDEE-46F1-B76C-117DD684DD75}" name="paradigm" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{4C03C951-46D8-47E8-8244-B52757673F4E}" name="notes" dataDxfId="2"/>
@@ -695,10 +797,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1073,6 +1175,166 @@
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
     </row>
+    <row r="33" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>